<commit_message>
feature_engineering was updated with group names
</commit_message>
<xml_diff>
--- a/Data_preparation/Feature_engineering.xlsx
+++ b/Data_preparation/Feature_engineering.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ML_project\Data_preparation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="גיליון1"/>
+    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">גיליון1!$A$1:$C$80</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
   <si>
     <t>Discharge disposition</t>
   </si>
@@ -46,9 +54,6 @@
     <t>Discharged/transferred to home with home health service</t>
   </si>
   <si>
-    <t>home care</t>
-  </si>
-  <si>
     <t>Left AMA</t>
   </si>
   <si>
@@ -284,18 +289,26 @@
   </si>
   <si>
     <t>Uncontrolled</t>
+  </si>
+  <si>
+    <t>discharged_home</t>
+  </si>
+  <si>
+    <t>Left_AMA</t>
+  </si>
+  <si>
+    <t>home_care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -320,13 +333,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -340,7 +353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdeebf7"/>
+        <fgColor rgb="FFDEEBF7"/>
       </patternFill>
     </fill>
   </fills>
@@ -354,13 +367,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -385,16 +398,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -402,77 +415,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -483,10 +498,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -524,71 +539,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -616,7 +631,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -639,11 +654,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -652,13 +667,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -668,7 +683,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -677,7 +692,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -686,7 +701,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -694,10 +709,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -768,16 +783,18 @@
   </sheetPr>
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="19" width="82.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="20" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="19" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="82.09765625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,16 +805,18 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="C2" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -808,34 +827,40 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -843,232 +868,264 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="C8" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="C9" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="5">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5">
-        <v>5</v>
-      </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" s="5">
-        <v>2</v>
-      </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="B17" s="5">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="B18" s="5">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5">
         <v>7</v>
       </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="C19" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="7" t="s">
+      <c r="B21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="7" t="s">
+      <c r="B22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="5">
-        <v>2</v>
-      </c>
-      <c r="C23" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="5">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B25" s="5">
-        <v>2</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="B26" s="5">
         <v>7</v>
       </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="C26" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="5">
         <v>7</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="C27" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="5">
-        <v>2</v>
-      </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="5">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="5">
-        <v>2</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="5">
-        <v>2</v>
-      </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="9" t="s">
+      <c r="B31" s="10">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="B31" s="10">
-        <v>2</v>
-      </c>
-      <c r="C31" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>1</v>
@@ -1077,83 +1134,97 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
       </c>
-      <c r="C33" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="C33" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="B34" s="5">
-        <v>2</v>
-      </c>
-      <c r="C34" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="B35" s="5">
         <v>3</v>
       </c>
-      <c r="C35" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="C35" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="5">
         <v>4</v>
       </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="C36" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="5">
+        <v>5</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="5">
-        <v>5</v>
-      </c>
-      <c r="C37" s="6" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="5">
-        <v>5</v>
-      </c>
-      <c r="C38" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="B39" s="5">
         <v>6</v>
       </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="C39" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="10">
         <v>5</v>
       </c>
-      <c r="C40" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="C40" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>1</v>
@@ -1162,244 +1233,282 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="5">
         <v>1</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="15" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
       </c>
-      <c r="C43" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="C43" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
       </c>
-      <c r="C44" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="C44" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="5">
+        <v>2</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="5">
-        <v>2</v>
-      </c>
-      <c r="C45" s="6" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="15" t="s">
+      <c r="B46" s="5">
+        <v>2</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="5">
-        <v>2</v>
-      </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="15" t="s">
+      <c r="B47" s="5">
+        <v>2</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="5">
-        <v>2</v>
-      </c>
-      <c r="C47" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="15" t="s">
+      <c r="B48" s="5">
+        <v>2</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="B48" s="5">
-        <v>2</v>
-      </c>
-      <c r="C48" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="15" t="s">
-        <v>55</v>
       </c>
       <c r="B49" s="5">
         <v>3</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="5">
         <v>4</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="5">
+        <v>2</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="5">
-        <v>2</v>
-      </c>
-      <c r="C51" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="15" t="s">
+      <c r="B52" s="5">
+        <v>5</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="5">
-        <v>5</v>
-      </c>
-      <c r="C52" s="6" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="15" t="s">
+      <c r="B53" s="5">
+        <v>5</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="5">
-        <v>5</v>
-      </c>
-      <c r="C53" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="15" t="s">
+      <c r="B54" s="5">
+        <v>5</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="5">
-        <v>5</v>
-      </c>
-      <c r="C54" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="15" t="s">
-        <v>62</v>
-      </c>
       <c r="B55" s="5">
         <v>5</v>
       </c>
-      <c r="C55" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="C55" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56" s="5">
         <v>4</v>
       </c>
-      <c r="C56" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="C56" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B57" s="5">
         <v>4</v>
       </c>
-      <c r="C57" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="C57" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="5">
+        <v>2</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="5">
-        <v>2</v>
-      </c>
-      <c r="C58" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="15" t="s">
-        <v>64</v>
-      </c>
       <c r="B59" s="5">
         <v>2</v>
       </c>
-      <c r="C59" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="C59" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B60" s="5">
         <v>4</v>
       </c>
-      <c r="C60" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="C60" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B61" s="5">
         <v>4</v>
       </c>
-      <c r="C61" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="C61" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="5">
+        <v>2</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="5">
-        <v>2</v>
-      </c>
-      <c r="C62" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="15" t="s">
+      <c r="B63" s="5">
+        <v>5</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="5">
-        <v>5</v>
-      </c>
-      <c r="C63" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="15" t="s">
+      <c r="B64" s="5">
+        <v>5</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="5">
-        <v>5</v>
-      </c>
-      <c r="C64" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="15" t="s">
+      <c r="B65" s="5">
+        <v>2</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="5">
-        <v>2</v>
-      </c>
-      <c r="C65" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="17" t="s">
+      <c r="B66" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="17"/>
+    </row>
+    <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>1</v>
@@ -1408,107 +1517,119 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" s="5">
         <v>1</v>
       </c>
       <c r="C68" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="15" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="15" t="s">
+      <c r="B69" s="5">
+        <v>2</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="5">
-        <v>2</v>
-      </c>
-      <c r="C69" s="4" t="s">
+    </row>
+    <row r="70" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="15" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="15" t="s">
-        <v>75</v>
       </c>
       <c r="B70" s="5">
         <v>3</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="15" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="15" t="s">
-        <v>77</v>
       </c>
       <c r="B71" s="5">
         <v>3</v>
       </c>
-      <c r="C71" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+      <c r="C71" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="5">
         <v>3</v>
       </c>
-      <c r="C72" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+      <c r="C72" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="5">
         <v>3</v>
       </c>
-      <c r="C73" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+      <c r="C73" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B74" s="5">
         <v>3</v>
       </c>
-      <c r="C74" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+      <c r="C74" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="5">
         <v>4</v>
       </c>
       <c r="C75" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="15" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="B76" s="5">
         <v>4</v>
       </c>
-      <c r="C76" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+      <c r="C76" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B77" s="10">
         <v>4</v>
       </c>
-      <c r="C77" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+      <c r="C77" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B78" s="16" t="s">
         <v>1</v>
@@ -1517,29 +1638,30 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row r="79" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" s="5">
         <v>1</v>
       </c>
       <c r="C79" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="15" t="s">
+      <c r="B80" s="5">
+        <v>2</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B80" s="5">
-        <v>2</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>89</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C80"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>